<commit_message>
Fixed the back button error
</commit_message>
<xml_diff>
--- a/uploads/Book1.xlsx
+++ b/uploads/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\College Stuff\Final Year IT Project\Test File\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{821761D6-DCAA-4E8C-BDFF-69DF6EA8D2EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF436A8-6675-474F-90D2-3B34D1CA34C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BF3C0583-5FB1-409A-804B-50F677D7444A}"/>
   </bookViews>
@@ -37,12 +37,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>BATCH</t>
   </si>
   <si>
     <t>DEFECTS</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Defect Type</t>
   </si>
 </sst>
 </file>
@@ -394,60 +400,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D557C15F-0A59-46B8-9BEE-D08FE3E2FD0F}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>